<commit_message>
reading excel files/parsing header updated README.md to include excel instructions
</commit_message>
<xml_diff>
--- a/bad-xlsx-input.xlsx
+++ b/bad-xlsx-input.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -265,11 +266,11 @@
   </sheetPr>
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="69" zoomScaleNormal="69" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.24"/>
@@ -463,4 +464,27 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
convert xlsx to yml function works correctly
</commit_message>
<xml_diff>
--- a/bad-xlsx-input.xlsx
+++ b/bad-xlsx-input.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -266,8 +266,8 @@
   </sheetPr>
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -473,7 +473,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>

</xml_diff>